<commit_message>
Documentação das classes da estrutura dos dados e acesso aos dados
</commit_message>
<xml_diff>
--- a/EuroTour/src/main/java/ifsc/edu/br/eurotour/datasource/Planilha de Países-Capitais Ordenada.xlsx
+++ b/EuroTour/src/main/java/ifsc/edu/br/eurotour/datasource/Planilha de Países-Capitais Ordenada.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\IFSC\1_Ensino\Ciência da Computação\3. Inteligência Artificial\2017-2\Trabalho de Busca\Alunos\IAMetodosDeBusca\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DFFD9CCD3090CC42D197F1854AEADBE53AC0DEFB" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{3CA4684B-2F95-47AE-B7EB-3D893B57B2A5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C122D566-DD11-4D4D-B9AB-3A826FBC88F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Reais" sheetId="1" r:id="rId1"/>
     <sheet name="Dados de Eurística" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -314,13 +310,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -607,8 +603,8 @@
   </sheetPr>
   <dimension ref="A1:AT47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -665,56 +661,56 @@
       <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
     </row>
     <row r="2" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="5" t="s">

</xml_diff>